<commit_message>
Final v0.3 flight version
</commit_message>
<xml_diff>
--- a/Flight_LOG_VEGA.xlsx
+++ b/Flight_LOG_VEGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem\Documents\Arduino_projects\Karman_Line\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46847B6B-2B4F-44B4-94DE-C0E90F2DC69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5157FFC2-B47E-4828-B1E4-CDE896E671D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{289AF73A-A276-495D-9D29-F73829A1D8C9}"/>
   </bookViews>
@@ -368,30 +368,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -402,6 +378,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -419,11 +398,32 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -21094,9 +21094,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6CFB9EE-5A60-4B26-9634-23E93BD7A1E6}" name="Telemetry_flight_LOG_VEGA_team" displayName="Telemetry_flight_LOG_VEGA_team" ref="A1:P541" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:P541" xr:uid="{E6CFB9EE-5A60-4B26-9634-23E93BD7A1E6}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{43F5D2C1-5750-4CED-8C06-ED1516E3B699}" uniqueName="1" name="Time" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{43F5D2C1-5750-4CED-8C06-ED1516E3B699}" uniqueName="1" name="Time" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{F7248654-B8A7-45AF-BB31-BB71954CA40B}" uniqueName="2" name="Temp" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{E0393775-8642-4A57-9C31-DA53104D97B0}" uniqueName="3" name="Height_K" queryTableFieldId="3" dataDxfId="1" dataCellStyle="Финансовый"/>
+    <tableColumn id="3" xr3:uid="{E0393775-8642-4A57-9C31-DA53104D97B0}" uniqueName="3" name="Height_K" queryTableFieldId="3" dataDxfId="0" dataCellStyle="Финансовый"/>
     <tableColumn id="4" xr3:uid="{7B7B1742-E3BC-4679-B144-00EDF35F6AD6}" uniqueName="4" name="VertSpeed" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{DBD5A252-5A0D-40AD-BD64-A63EFFDF7BC0}" uniqueName="5" name="accel_X" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{C7DFBC5E-BE0B-43F9-A9E6-7A396DD6DC12}" uniqueName="6" name="accel_Y" queryTableFieldId="6"/>
@@ -25923,19 +25923,19 @@
         <v>184.26</v>
       </c>
       <c r="Q88" s="1"/>
-      <c r="R88" s="5" t="s">
+      <c r="R88" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="5"/>
-      <c r="V88" s="6">
+      <c r="S88" s="21"/>
+      <c r="T88" s="21"/>
+      <c r="U88" s="21"/>
+      <c r="V88" s="19">
         <f>A138</f>
         <v>50.331000000000003</v>
       </c>
-      <c r="W88" s="7"/>
-      <c r="X88" s="7"/>
-      <c r="Y88" s="9" t="s">
+      <c r="W88" s="14"/>
+      <c r="X88" s="14"/>
+      <c r="Y88" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -25989,14 +25989,14 @@
         <v>191.49</v>
       </c>
       <c r="Q89" s="1"/>
-      <c r="R89" s="5"/>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="5"/>
-      <c r="V89" s="8"/>
-      <c r="W89" s="7"/>
-      <c r="X89" s="7"/>
-      <c r="Y89" s="4"/>
+      <c r="R89" s="21"/>
+      <c r="S89" s="21"/>
+      <c r="T89" s="21"/>
+      <c r="U89" s="21"/>
+      <c r="V89" s="20"/>
+      <c r="W89" s="14"/>
+      <c r="X89" s="14"/>
+      <c r="Y89" s="17"/>
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
@@ -26048,14 +26048,14 @@
         <v>191.49</v>
       </c>
       <c r="Q90" s="1"/>
-      <c r="R90" s="5"/>
-      <c r="S90" s="5"/>
-      <c r="T90" s="5"/>
-      <c r="U90" s="5"/>
-      <c r="V90" s="8"/>
-      <c r="W90" s="7"/>
-      <c r="X90" s="7"/>
-      <c r="Y90" s="4"/>
+      <c r="R90" s="21"/>
+      <c r="S90" s="21"/>
+      <c r="T90" s="21"/>
+      <c r="U90" s="21"/>
+      <c r="V90" s="20"/>
+      <c r="W90" s="14"/>
+      <c r="X90" s="14"/>
+      <c r="Y90" s="17"/>
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
@@ -26107,19 +26107,19 @@
         <v>191.49</v>
       </c>
       <c r="Q91" s="1"/>
-      <c r="R91" s="5" t="s">
+      <c r="R91" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="S91" s="5"/>
-      <c r="T91" s="5"/>
-      <c r="U91" s="5"/>
-      <c r="V91" s="6">
+      <c r="S91" s="21"/>
+      <c r="T91" s="21"/>
+      <c r="U91" s="21"/>
+      <c r="V91" s="19">
         <f>A20</f>
         <v>6.5449999999999999</v>
       </c>
-      <c r="W91" s="7"/>
-      <c r="X91" s="7"/>
-      <c r="Y91" s="9" t="s">
+      <c r="W91" s="14"/>
+      <c r="X91" s="14"/>
+      <c r="Y91" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -26173,14 +26173,14 @@
         <v>198.11</v>
       </c>
       <c r="Q92" s="1"/>
-      <c r="R92" s="5"/>
-      <c r="S92" s="5"/>
-      <c r="T92" s="5"/>
-      <c r="U92" s="5"/>
-      <c r="V92" s="8"/>
-      <c r="W92" s="7"/>
-      <c r="X92" s="7"/>
-      <c r="Y92" s="4"/>
+      <c r="R92" s="21"/>
+      <c r="S92" s="21"/>
+      <c r="T92" s="21"/>
+      <c r="U92" s="21"/>
+      <c r="V92" s="20"/>
+      <c r="W92" s="14"/>
+      <c r="X92" s="14"/>
+      <c r="Y92" s="17"/>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
@@ -26232,14 +26232,14 @@
         <v>198.11</v>
       </c>
       <c r="Q93" s="1"/>
-      <c r="R93" s="5"/>
-      <c r="S93" s="5"/>
-      <c r="T93" s="5"/>
-      <c r="U93" s="5"/>
-      <c r="V93" s="8"/>
-      <c r="W93" s="7"/>
-      <c r="X93" s="7"/>
-      <c r="Y93" s="4"/>
+      <c r="R93" s="21"/>
+      <c r="S93" s="21"/>
+      <c r="T93" s="21"/>
+      <c r="U93" s="21"/>
+      <c r="V93" s="20"/>
+      <c r="W93" s="14"/>
+      <c r="X93" s="14"/>
+      <c r="Y93" s="17"/>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
@@ -26291,19 +26291,19 @@
         <v>202.62</v>
       </c>
       <c r="Q94" s="1"/>
-      <c r="R94" s="5" t="s">
+      <c r="R94" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="S94" s="5"/>
-      <c r="T94" s="5"/>
-      <c r="U94" s="5"/>
-      <c r="V94" s="6">
+      <c r="S94" s="21"/>
+      <c r="T94" s="21"/>
+      <c r="U94" s="21"/>
+      <c r="V94" s="19">
         <f>MAX(Telemetry_flight_LOG_VEGA_team[Height_K])</f>
         <v>206.74799999999999</v>
       </c>
-      <c r="W94" s="7"/>
-      <c r="X94" s="7"/>
-      <c r="Y94" s="9" t="s">
+      <c r="W94" s="14"/>
+      <c r="X94" s="14"/>
+      <c r="Y94" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -26357,14 +26357,14 @@
         <v>202.62</v>
       </c>
       <c r="Q95" s="1"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="8"/>
-      <c r="W95" s="7"/>
-      <c r="X95" s="7"/>
-      <c r="Y95" s="4"/>
+      <c r="R95" s="21"/>
+      <c r="S95" s="21"/>
+      <c r="T95" s="21"/>
+      <c r="U95" s="21"/>
+      <c r="V95" s="20"/>
+      <c r="W95" s="14"/>
+      <c r="X95" s="14"/>
+      <c r="Y95" s="17"/>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
@@ -26416,14 +26416,14 @@
         <v>202.62</v>
       </c>
       <c r="Q96" s="1"/>
-      <c r="R96" s="5"/>
-      <c r="S96" s="5"/>
-      <c r="T96" s="5"/>
-      <c r="U96" s="5"/>
-      <c r="V96" s="8"/>
-      <c r="W96" s="7"/>
-      <c r="X96" s="7"/>
-      <c r="Y96" s="4"/>
+      <c r="R96" s="21"/>
+      <c r="S96" s="21"/>
+      <c r="T96" s="21"/>
+      <c r="U96" s="21"/>
+      <c r="V96" s="20"/>
+      <c r="W96" s="14"/>
+      <c r="X96" s="14"/>
+      <c r="Y96" s="17"/>
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
@@ -26475,19 +26475,19 @@
         <v>207.26</v>
       </c>
       <c r="Q97" s="1"/>
-      <c r="R97" s="5" t="s">
+      <c r="R97" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S97" s="5"/>
-      <c r="T97" s="5"/>
-      <c r="U97" s="5"/>
-      <c r="V97" s="6">
+      <c r="S97" s="21"/>
+      <c r="T97" s="21"/>
+      <c r="U97" s="21"/>
+      <c r="V97" s="19">
         <f>P541</f>
         <v>228.43</v>
       </c>
-      <c r="W97" s="7"/>
-      <c r="X97" s="7"/>
-      <c r="Y97" s="9" t="s">
+      <c r="W97" s="14"/>
+      <c r="X97" s="14"/>
+      <c r="Y97" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -26541,14 +26541,14 @@
         <v>207.26</v>
       </c>
       <c r="Q98" s="1"/>
-      <c r="R98" s="5"/>
-      <c r="S98" s="5"/>
-      <c r="T98" s="5"/>
-      <c r="U98" s="5"/>
-      <c r="V98" s="8"/>
-      <c r="W98" s="7"/>
-      <c r="X98" s="7"/>
-      <c r="Y98" s="4"/>
+      <c r="R98" s="21"/>
+      <c r="S98" s="21"/>
+      <c r="T98" s="21"/>
+      <c r="U98" s="21"/>
+      <c r="V98" s="20"/>
+      <c r="W98" s="14"/>
+      <c r="X98" s="14"/>
+      <c r="Y98" s="17"/>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
@@ -26600,14 +26600,14 @@
         <v>207.26</v>
       </c>
       <c r="Q99" s="1"/>
-      <c r="R99" s="11"/>
-      <c r="S99" s="11"/>
-      <c r="T99" s="11"/>
-      <c r="U99" s="11"/>
-      <c r="V99" s="8"/>
-      <c r="W99" s="7"/>
-      <c r="X99" s="7"/>
-      <c r="Y99" s="4"/>
+      <c r="R99" s="22"/>
+      <c r="S99" s="22"/>
+      <c r="T99" s="22"/>
+      <c r="U99" s="22"/>
+      <c r="V99" s="20"/>
+      <c r="W99" s="14"/>
+      <c r="X99" s="14"/>
+      <c r="Y99" s="17"/>
     </row>
     <row r="100" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
@@ -26659,19 +26659,19 @@
         <v>213.75</v>
       </c>
       <c r="Q100" s="1"/>
-      <c r="R100" s="12" t="s">
+      <c r="R100" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S100" s="13"/>
-      <c r="T100" s="13"/>
-      <c r="U100" s="14"/>
-      <c r="V100" s="6">
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="6"/>
+      <c r="V100" s="19">
         <f>MAX(Telemetry_flight_LOG_VEGA_team[VertSpeed])</f>
         <v>93.7</v>
       </c>
-      <c r="W100" s="7"/>
-      <c r="X100" s="7"/>
-      <c r="Y100" s="9" t="s">
+      <c r="W100" s="14"/>
+      <c r="X100" s="14"/>
+      <c r="Y100" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -26725,14 +26725,14 @@
         <v>213.75</v>
       </c>
       <c r="Q101" s="1"/>
-      <c r="R101" s="15"/>
-      <c r="S101" s="10"/>
-      <c r="T101" s="10"/>
-      <c r="U101" s="16"/>
-      <c r="V101" s="8"/>
-      <c r="W101" s="7"/>
-      <c r="X101" s="7"/>
-      <c r="Y101" s="9"/>
+      <c r="R101" s="7"/>
+      <c r="S101" s="8"/>
+      <c r="T101" s="8"/>
+      <c r="U101" s="9"/>
+      <c r="V101" s="20"/>
+      <c r="W101" s="14"/>
+      <c r="X101" s="14"/>
+      <c r="Y101" s="16"/>
     </row>
     <row r="102" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
@@ -26784,14 +26784,14 @@
         <v>218.47</v>
       </c>
       <c r="Q102" s="1"/>
-      <c r="R102" s="15"/>
-      <c r="S102" s="10"/>
-      <c r="T102" s="10"/>
-      <c r="U102" s="16"/>
-      <c r="V102" s="8"/>
-      <c r="W102" s="7"/>
-      <c r="X102" s="7"/>
-      <c r="Y102" s="9"/>
+      <c r="R102" s="7"/>
+      <c r="S102" s="8"/>
+      <c r="T102" s="8"/>
+      <c r="U102" s="9"/>
+      <c r="V102" s="20"/>
+      <c r="W102" s="14"/>
+      <c r="X102" s="14"/>
+      <c r="Y102" s="16"/>
     </row>
     <row r="103" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
@@ -26843,14 +26843,14 @@
         <v>218.47</v>
       </c>
       <c r="Q103" s="1"/>
-      <c r="R103" s="17"/>
-      <c r="S103" s="18"/>
-      <c r="T103" s="18"/>
-      <c r="U103" s="19"/>
-      <c r="V103" s="6"/>
-      <c r="W103" s="7"/>
-      <c r="X103" s="7"/>
-      <c r="Y103" s="9"/>
+      <c r="R103" s="10"/>
+      <c r="S103" s="11"/>
+      <c r="T103" s="11"/>
+      <c r="U103" s="12"/>
+      <c r="V103" s="19"/>
+      <c r="W103" s="14"/>
+      <c r="X103" s="14"/>
+      <c r="Y103" s="16"/>
     </row>
     <row r="104" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
@@ -26902,19 +26902,19 @@
         <v>218.47</v>
       </c>
       <c r="Q104" s="1"/>
-      <c r="R104" s="12" t="s">
+      <c r="R104" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S104" s="13"/>
-      <c r="T104" s="13"/>
-      <c r="U104" s="14"/>
-      <c r="V104" s="20">
+      <c r="S104" s="5"/>
+      <c r="T104" s="5"/>
+      <c r="U104" s="6"/>
+      <c r="V104" s="13">
         <f>MAX(Telemetry_flight_LOG_VEGA_team[Sp])</f>
         <v>14.52</v>
       </c>
-      <c r="W104" s="7"/>
-      <c r="X104" s="7"/>
-      <c r="Y104" s="9" t="s">
+      <c r="W104" s="14"/>
+      <c r="X104" s="14"/>
+      <c r="Y104" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -26968,14 +26968,14 @@
         <v>225.42</v>
       </c>
       <c r="Q105" s="1"/>
-      <c r="R105" s="15"/>
-      <c r="S105" s="10"/>
-      <c r="T105" s="10"/>
-      <c r="U105" s="16"/>
-      <c r="V105" s="21"/>
-      <c r="W105" s="7"/>
-      <c r="X105" s="7"/>
-      <c r="Y105" s="4"/>
+      <c r="R105" s="7"/>
+      <c r="S105" s="8"/>
+      <c r="T105" s="8"/>
+      <c r="U105" s="9"/>
+      <c r="V105" s="15"/>
+      <c r="W105" s="14"/>
+      <c r="X105" s="14"/>
+      <c r="Y105" s="17"/>
     </row>
     <row r="106" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
@@ -27027,14 +27027,14 @@
         <v>225.42</v>
       </c>
       <c r="Q106" s="1"/>
-      <c r="R106" s="15"/>
-      <c r="S106" s="10"/>
-      <c r="T106" s="10"/>
-      <c r="U106" s="16"/>
-      <c r="V106" s="21"/>
-      <c r="W106" s="7"/>
-      <c r="X106" s="7"/>
-      <c r="Y106" s="4"/>
+      <c r="R106" s="7"/>
+      <c r="S106" s="8"/>
+      <c r="T106" s="8"/>
+      <c r="U106" s="9"/>
+      <c r="V106" s="15"/>
+      <c r="W106" s="14"/>
+      <c r="X106" s="14"/>
+      <c r="Y106" s="17"/>
     </row>
     <row r="107" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
@@ -27086,10 +27086,10 @@
         <v>225.42</v>
       </c>
       <c r="Q107" s="1"/>
-      <c r="R107" s="17"/>
-      <c r="S107" s="18"/>
-      <c r="T107" s="18"/>
-      <c r="U107" s="19"/>
+      <c r="R107" s="10"/>
+      <c r="S107" s="11"/>
+      <c r="T107" s="11"/>
+      <c r="U107" s="12"/>
     </row>
     <row r="108" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
@@ -27141,19 +27141,19 @@
         <v>231.78</v>
       </c>
       <c r="Q108" s="1"/>
-      <c r="R108" s="22" t="s">
+      <c r="R108" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="S108" s="13"/>
-      <c r="T108" s="13"/>
-      <c r="U108" s="14"/>
-      <c r="V108" s="20" cm="1">
+      <c r="S108" s="5"/>
+      <c r="T108" s="5"/>
+      <c r="U108" s="6"/>
+      <c r="V108" s="13" cm="1">
         <f t="array" ref="V108">MAX(ABS(Telemetry_flight_LOG_VEGA_team[[accel_X]:[accel_Z]]))</f>
         <v>7.67</v>
       </c>
-      <c r="W108" s="7"/>
-      <c r="X108" s="7"/>
-      <c r="Y108" s="9" t="s">
+      <c r="W108" s="14"/>
+      <c r="X108" s="14"/>
+      <c r="Y108" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -27207,14 +27207,14 @@
         <v>231.78</v>
       </c>
       <c r="Q109" s="1"/>
-      <c r="R109" s="15"/>
-      <c r="S109" s="10"/>
-      <c r="T109" s="10"/>
-      <c r="U109" s="16"/>
-      <c r="V109" s="21"/>
-      <c r="W109" s="7"/>
-      <c r="X109" s="7"/>
-      <c r="Y109" s="4"/>
+      <c r="R109" s="7"/>
+      <c r="S109" s="8"/>
+      <c r="T109" s="8"/>
+      <c r="U109" s="9"/>
+      <c r="V109" s="15"/>
+      <c r="W109" s="14"/>
+      <c r="X109" s="14"/>
+      <c r="Y109" s="17"/>
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
@@ -27266,14 +27266,14 @@
         <v>238.57</v>
       </c>
       <c r="Q110" s="1"/>
-      <c r="R110" s="15"/>
-      <c r="S110" s="10"/>
-      <c r="T110" s="10"/>
-      <c r="U110" s="16"/>
-      <c r="V110" s="21"/>
-      <c r="W110" s="7"/>
-      <c r="X110" s="7"/>
-      <c r="Y110" s="4"/>
+      <c r="R110" s="7"/>
+      <c r="S110" s="8"/>
+      <c r="T110" s="8"/>
+      <c r="U110" s="9"/>
+      <c r="V110" s="15"/>
+      <c r="W110" s="14"/>
+      <c r="X110" s="14"/>
+      <c r="Y110" s="17"/>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
@@ -27325,19 +27325,19 @@
         <v>238.57</v>
       </c>
       <c r="Q111" s="1"/>
-      <c r="R111" s="12" t="s">
+      <c r="R111" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S111" s="13"/>
-      <c r="T111" s="13"/>
-      <c r="U111" s="14"/>
-      <c r="V111" s="20">
+      <c r="S111" s="5"/>
+      <c r="T111" s="5"/>
+      <c r="U111" s="6"/>
+      <c r="V111" s="13">
         <f>(MAX(M3:M541))-(MIN(M3:M541))</f>
         <v>200.4</v>
       </c>
-      <c r="W111" s="7"/>
-      <c r="X111" s="7"/>
-      <c r="Y111" s="9" t="s">
+      <c r="W111" s="14"/>
+      <c r="X111" s="14"/>
+      <c r="Y111" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -27391,14 +27391,14 @@
         <v>238.57</v>
       </c>
       <c r="Q112" s="1"/>
-      <c r="R112" s="15"/>
-      <c r="S112" s="10"/>
-      <c r="T112" s="10"/>
-      <c r="U112" s="16"/>
-      <c r="V112" s="21"/>
-      <c r="W112" s="7"/>
-      <c r="X112" s="7"/>
-      <c r="Y112" s="4"/>
+      <c r="R112" s="7"/>
+      <c r="S112" s="8"/>
+      <c r="T112" s="8"/>
+      <c r="U112" s="9"/>
+      <c r="V112" s="15"/>
+      <c r="W112" s="14"/>
+      <c r="X112" s="14"/>
+      <c r="Y112" s="17"/>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
@@ -27450,14 +27450,14 @@
         <v>244.28</v>
       </c>
       <c r="Q113" s="1"/>
-      <c r="R113" s="17"/>
-      <c r="S113" s="18"/>
-      <c r="T113" s="18"/>
-      <c r="U113" s="19"/>
-      <c r="V113" s="21"/>
-      <c r="W113" s="7"/>
-      <c r="X113" s="7"/>
-      <c r="Y113" s="4"/>
+      <c r="R113" s="10"/>
+      <c r="S113" s="11"/>
+      <c r="T113" s="11"/>
+      <c r="U113" s="12"/>
+      <c r="V113" s="15"/>
+      <c r="W113" s="14"/>
+      <c r="X113" s="14"/>
+      <c r="Y113" s="17"/>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
@@ -49289,15 +49289,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R111:U113"/>
-    <mergeCell ref="V111:X113"/>
-    <mergeCell ref="Y111:Y113"/>
-    <mergeCell ref="V104:X106"/>
-    <mergeCell ref="Y104:Y106"/>
-    <mergeCell ref="R104:U107"/>
-    <mergeCell ref="R108:U110"/>
-    <mergeCell ref="V108:X110"/>
-    <mergeCell ref="Y108:Y110"/>
+    <mergeCell ref="R88:U90"/>
+    <mergeCell ref="V88:X90"/>
+    <mergeCell ref="Y88:Y90"/>
+    <mergeCell ref="R91:U93"/>
+    <mergeCell ref="V91:X93"/>
+    <mergeCell ref="Y91:Y93"/>
     <mergeCell ref="V100:X102"/>
     <mergeCell ref="R100:U103"/>
     <mergeCell ref="Y100:Y103"/>
@@ -49308,12 +49305,15 @@
     <mergeCell ref="R97:U99"/>
     <mergeCell ref="V97:X99"/>
     <mergeCell ref="Y97:Y99"/>
-    <mergeCell ref="R88:U90"/>
-    <mergeCell ref="V88:X90"/>
-    <mergeCell ref="Y88:Y90"/>
-    <mergeCell ref="R91:U93"/>
-    <mergeCell ref="V91:X93"/>
-    <mergeCell ref="Y91:Y93"/>
+    <mergeCell ref="R111:U113"/>
+    <mergeCell ref="V111:X113"/>
+    <mergeCell ref="Y111:Y113"/>
+    <mergeCell ref="V104:X106"/>
+    <mergeCell ref="Y104:Y106"/>
+    <mergeCell ref="R104:U107"/>
+    <mergeCell ref="R108:U110"/>
+    <mergeCell ref="V108:X110"/>
+    <mergeCell ref="Y108:Y110"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>